<commit_message>
modulos de cadastro de segmento, secao e especie
</commit_message>
<xml_diff>
--- a/Cadastros Auto Nextt limpa.xlsx
+++ b/Cadastros Auto Nextt limpa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Desktop\dev\automacao-nextt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard\Desktop\dev\automacao-nextt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BD050B-112B-404A-B833-25F09FD3B81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B05C3A-F29A-4709-87A1-A8E724D756A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="764" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21390" tabRatio="764" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nextt" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="Cadastro de Espécie" sheetId="7" r:id="rId7"/>
     <sheet name="Dados Consolidados" sheetId="5" r:id="rId8"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
   <definedNames>
     <definedName name="Seção1">#REF!</definedName>
     <definedName name="Seção2">#REF!</definedName>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
   <si>
     <t>Cadastre vários itens simultaneamente</t>
   </si>
@@ -221,9 +224,6 @@
   </si>
   <si>
     <t>Este tipo de cadastro funciona de maneira similar à Matriz: você pode selecionar as informações diretamente de nossos bancos de dados e cadastrar seus produtos, pedidos, marcas e muito mais de forma automática. O melhor de tudo é que esse processo pode ser realizado em lotes, tornando tudo mais ágil e eficiente.</t>
-  </si>
-  <si>
-    <t>CNPJ</t>
   </si>
   <si>
     <t>Máximo 50 caracteres. As descrições de "seção" serão consideradas válidas apenas se forem diferentes das já existentes no banco de dados do Matriz</t>
@@ -1044,17 +1044,23 @@
     <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1079,12 +1085,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1155,108 +1155,309 @@
 </styleSheet>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="495300" cy="495300"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image2.png" title="Imagen">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3BD39E7-863C-4BAC-94FD-AF6BAE1CBBB2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5391150" y="1771650"/>
-          <a:ext cx="495300" cy="495300"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>494826</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2" descr="Nextt Soluções">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A36CE6C-B1A7-D444-FDCE-C0A971006217}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="285750" y="76200"/>
-          <a:ext cx="1428276" cy="685799"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>12544425</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Button 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F5A55E6-8B18-EF0A-7C63-4438F6FAD850}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                  <a:cs typeface="Calibri"/>
+                </a:rPr>
+                <a:t>Cadastrar</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2049" name="Button 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C958E15E-5A00-ABE4-1ED5-ABE98EEDB277}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                  <a:cs typeface="Calibri"/>
+                </a:rPr>
+                <a:t>Cadastrar</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3073" name="Button 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3073"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7969BF53-F9A7-9AA8-9427-DAC5761D144F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                  <a:cs typeface="Calibri"/>
+                </a:rPr>
+                <a:t>Cadastrar</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Nextt"/>
+      <sheetName val="Cadastro de Produtos"/>
+      <sheetName val="Cadastro de Pedidos"/>
+      <sheetName val="Cadastro de Marcas"/>
+      <sheetName val="Cadastro de Segmento"/>
+      <sheetName val="Cadastro de Seção"/>
+      <sheetName val="Cadastro de Espécie"/>
+      <sheetName val="Dados Consolidados"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="ExecutarCadastroEspecie"/>
+      <definedName name="ExecutarCadastroSecao"/>
+      <definedName name="ExecutarCadastroSegmento"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1559,7 +1760,9 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1625,70 +1828,70 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="69"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
-      <c r="O4" s="68"/>
+      <c r="A4" s="72"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
     </row>
     <row r="5" spans="1:15" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="67"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="68"/>
+      <c r="A5" s="71"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
     </row>
     <row r="6" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="69"/>
     </row>
     <row r="7" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="68"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="71" t="s">
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -1698,11 +1901,11 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -1715,13 +1918,13 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="68"/>
+      <c r="C9" s="69"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -1734,34 +1937,34 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="68"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="75" t="s">
+      <c r="H10" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="68"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="68"/>
-      <c r="L10" s="68"/>
-      <c r="M10" s="68"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="69"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="68"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="68"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -1777,8 +1980,8 @@
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="68"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1791,18 +1994,18 @@
     </row>
     <row r="13" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="68"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="71" t="s">
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
@@ -1812,11 +2015,11 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1829,60 +2032,60 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="81"/>
+      <c r="C15" s="67"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="82" t="s">
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="H15" s="82"/>
-      <c r="I15" s="82"/>
-      <c r="J15" s="82"/>
-      <c r="K15" s="82"/>
-      <c r="L15" s="82"/>
-      <c r="M15" s="82"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="70"/>
+      <c r="K15" s="70"/>
+      <c r="L15" s="70"/>
+      <c r="M15" s="70"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="81"/>
+      <c r="C16" s="67"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="82"/>
-      <c r="H16" s="82"/>
-      <c r="I16" s="82"/>
-      <c r="J16" s="82"/>
-      <c r="K16" s="82"/>
-      <c r="L16" s="82"/>
-      <c r="M16" s="82"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="81"/>
+      <c r="C17" s="67"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="82"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="82"/>
-      <c r="K17" s="82"/>
-      <c r="L17" s="82"/>
-      <c r="M17" s="82"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="70"/>
+      <c r="K17" s="70"/>
+      <c r="L17" s="70"/>
+      <c r="M17" s="70"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
@@ -1891,15 +2094,15 @@
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="82"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="82"/>
-      <c r="M18" s="82"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="70"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
@@ -1908,15 +2111,15 @@
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="82"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="82"/>
-      <c r="J19" s="82"/>
-      <c r="K19" s="82"/>
-      <c r="L19" s="82"/>
-      <c r="M19" s="82"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="70"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
@@ -1925,8 +2128,8 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1942,18 +2145,18 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="76" t="s">
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="77"/>
-      <c r="I21" s="77"/>
-      <c r="J21" s="77"/>
-      <c r="K21" s="77"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="77"/>
-      <c r="N21" s="77"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="79"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="79"/>
+      <c r="M21" s="79"/>
+      <c r="N21" s="79"/>
       <c r="O21" s="5"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1961,8 +2164,8 @@
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -1978,8 +2181,8 @@
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
       <c r="G23" s="32" t="s">
         <v>42</v>
       </c>
@@ -1997,8 +2200,8 @@
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -2014,17 +2217,17 @@
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
       <c r="G25" s="33"/>
-      <c r="H25" s="78" t="s">
+      <c r="H25" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="I25" s="79"/>
-      <c r="J25" s="79"/>
-      <c r="K25" s="79"/>
-      <c r="L25" s="79"/>
-      <c r="M25" s="79"/>
+      <c r="I25" s="81"/>
+      <c r="J25" s="81"/>
+      <c r="K25" s="81"/>
+      <c r="L25" s="81"/>
+      <c r="M25" s="81"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
     </row>
@@ -2033,15 +2236,15 @@
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="80"/>
-      <c r="I26" s="80"/>
-      <c r="J26" s="80"/>
-      <c r="K26" s="80"/>
-      <c r="L26" s="80"/>
-      <c r="M26" s="79"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="82"/>
+      <c r="J26" s="82"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="82"/>
+      <c r="M26" s="81"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
     </row>
@@ -2050,15 +2253,15 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="80"/>
-      <c r="I27" s="80"/>
-      <c r="J27" s="80"/>
-      <c r="K27" s="80"/>
-      <c r="L27" s="80"/>
-      <c r="M27" s="79"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="81"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
     </row>
@@ -2067,8 +2270,8 @@
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="68"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -2084,8 +2287,8 @@
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="68"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -2101,8 +2304,8 @@
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -2118,8 +2321,8 @@
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="68"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -2135,8 +2338,8 @@
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="68"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -2152,8 +2355,8 @@
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="68"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -2169,8 +2372,8 @@
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -2186,8 +2389,8 @@
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="68"/>
-      <c r="F35" s="68"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -2203,8 +2406,8 @@
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="68"/>
-      <c r="F36" s="68"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -2220,8 +2423,8 @@
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -2237,8 +2440,8 @@
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="68"/>
-      <c r="F38" s="68"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="69"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -2254,8 +2457,8 @@
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="68"/>
-      <c r="F39" s="68"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="69"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -2271,8 +2474,8 @@
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="68"/>
-      <c r="F40" s="68"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="69"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -2288,8 +2491,8 @@
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="68"/>
-      <c r="F41" s="68"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="69"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
@@ -2305,8 +2508,8 @@
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="68"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
@@ -2322,8 +2525,8 @@
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
-      <c r="E43" s="68"/>
-      <c r="F43" s="68"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="69"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
@@ -2339,8 +2542,8 @@
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
-      <c r="E44" s="68"/>
-      <c r="F44" s="68"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="69"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
@@ -2356,8 +2559,8 @@
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
-      <c r="E45" s="68"/>
-      <c r="F45" s="68"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="69"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
@@ -2373,8 +2576,8 @@
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
-      <c r="E46" s="68"/>
-      <c r="F46" s="68"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="69"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
@@ -2390,8 +2593,8 @@
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
-      <c r="E47" s="68"/>
-      <c r="F47" s="68"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="69"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -2407,8 +2610,8 @@
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
-      <c r="E48" s="68"/>
-      <c r="F48" s="68"/>
+      <c r="E48" s="69"/>
+      <c r="F48" s="69"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
@@ -2424,8 +2627,8 @@
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
-      <c r="E49" s="68"/>
-      <c r="F49" s="68"/>
+      <c r="E49" s="69"/>
+      <c r="F49" s="69"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
@@ -2441,8 +2644,8 @@
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-      <c r="E50" s="68"/>
-      <c r="F50" s="68"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="69"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
@@ -2456,11 +2659,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="21">
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G15:M19"/>
-    <mergeCell ref="B15:C15"/>
     <mergeCell ref="A5:O5"/>
     <mergeCell ref="A4:O4"/>
     <mergeCell ref="B9:C9"/>
@@ -2477,6 +2675,11 @@
     <mergeCell ref="H25:M27"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G15:M19"/>
+    <mergeCell ref="B15:C15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" location="'Cadastro de Produtos'!A1" display="Cadastro de Produtos" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2487,7 +2690,6 @@
     <hyperlink ref="B15:C15" location="'Cadastro de Segmento'!A1" display="Cadastro de Segmento" xr:uid="{9362759C-8C78-4D34-ADEA-62AC0184B4EF}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2531,9 +2733,9 @@
       <c r="A1" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -2570,9 +2772,9 @@
       <c r="A2" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -2751,10 +2953,10 @@
         <v>30</v>
       </c>
       <c r="C5" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="41" t="s">
         <v>64</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>65</v>
       </c>
       <c r="E5" s="40" t="s">
         <v>31</v>
@@ -2788,13 +2990,13 @@
       <c r="V5" s="41"/>
       <c r="W5" s="41"/>
       <c r="X5" s="41"/>
-      <c r="Y5" s="68"/>
-      <c r="Z5" s="68"/>
-      <c r="AA5" s="68"/>
-      <c r="AB5" s="68"/>
-      <c r="AC5" s="68"/>
-      <c r="AD5" s="68"/>
-      <c r="AE5" s="68"/>
+      <c r="Y5" s="69"/>
+      <c r="Z5" s="69"/>
+      <c r="AA5" s="69"/>
+      <c r="AB5" s="69"/>
+      <c r="AC5" s="69"/>
+      <c r="AD5" s="69"/>
+      <c r="AE5" s="69"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
@@ -2827,13 +3029,13 @@
       <c r="V6" s="47"/>
       <c r="W6" s="44"/>
       <c r="X6" s="47"/>
-      <c r="Y6" s="68"/>
-      <c r="Z6" s="68"/>
-      <c r="AA6" s="68"/>
-      <c r="AB6" s="68"/>
-      <c r="AC6" s="68"/>
-      <c r="AD6" s="68"/>
-      <c r="AE6" s="68"/>
+      <c r="Y6" s="69"/>
+      <c r="Z6" s="69"/>
+      <c r="AA6" s="69"/>
+      <c r="AB6" s="69"/>
+      <c r="AC6" s="69"/>
+      <c r="AD6" s="69"/>
+      <c r="AE6" s="69"/>
     </row>
     <row r="7" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="55"/>
@@ -19172,7 +19374,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19269,9 +19471,7 @@
       <c r="AD2" s="90"/>
     </row>
     <row r="3" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -19491,7 +19691,7 @@
     </row>
     <row r="5" spans="1:16" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -19513,15 +19713,15 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA2666A-C429-48B8-AED9-D06D5D5C6D1B}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA2666A-C429-48B8-AED9-D06D5D5C6D1B}">
+  <sheetPr codeName="Planilha6">
     <tabColor theme="2" tint="-0.749992370372631"/>
   </sheetPr>
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19578,7 +19778,7 @@
     </row>
     <row r="5" spans="1:13" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -19586,12 +19786,42 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId3" name="Button 2">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!ExecutarCadastroSegmento">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>12544425</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD76123E-B956-4C86-9056-36B82AC4C9D1}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD76123E-B956-4C86-9056-36B82AC4C9D1}">
+  <sheetPr codeName="Planilha7">
     <tabColor theme="2" tint="-0.749992370372631"/>
   </sheetPr>
   <dimension ref="A1:O200"/>
@@ -19599,14 +19829,14 @@
     <sheetView workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.5703125" customWidth="1"/>
     <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="176.28515625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -19676,7 +19906,7 @@
     </row>
     <row r="5" spans="1:15" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="40" t="s">
         <v>51</v>
@@ -19690,1165 +19920,1165 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B7, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B7, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B8, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B8, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B9, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B9, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C10" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B10, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B10, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B11, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B11, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B12, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B12, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B13, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B13, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C14" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B14, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B14, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B15, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B15, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B16, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B16, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B17, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B17, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B18, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B18, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B19, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B19, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B20, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B20, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B21, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B21, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B22, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B22, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B23, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B23, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B24, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B24, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B25, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B25, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B26, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B26, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B27, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B27, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B28, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B28, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B29, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B29, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B30, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B30, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B31, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B31, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B32, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B32, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B33, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B33, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B34, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B34, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B35, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B35, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B36, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B36, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B37, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B37, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B38, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B38, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B39, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B39, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B40, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B40, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B41, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B41, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B42, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B42, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B43, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B43, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B44, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B44, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B45, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B45, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B46, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B46, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B47, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B47, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B48, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B48, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B49, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B49, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B50, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B50, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B51, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B51, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B52, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B52, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B53, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B53, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B54, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B54, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B55, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B55, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B56, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B56, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B57, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B57, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B58, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B58, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B59, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B59, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B60, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B60, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B61, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B61, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B62, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B62, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B63, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B63, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B64, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B64, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B65, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B65, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B66, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B66, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B67, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B67, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B68, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B68, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B69, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B69, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B70, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B70, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B71, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B71, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B72, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B72, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B73, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B73, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B74, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B74, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B75, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B75, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B76, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B76, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B77, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B77, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B78, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B78, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B79, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B79, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B80, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B80, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B81, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B81, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B82, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B82, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B83, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B83, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B84, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B84, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B85, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B85, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C86" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B86, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B86, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B87, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B87, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C88" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B88, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B88, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B89, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B89, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C90" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B90, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B90, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B91, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B91, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C92" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B92, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B92, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B93, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B93, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C94" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B94, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B94, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B95, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B95, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C96" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B96, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B96, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B97, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B97, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C98" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B98, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B98, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B99, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B99, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C100" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B100, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B100, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B101, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B101, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C102" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B102, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B102, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C103" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B103, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B103, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C104" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B104, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B104, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C105" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B105, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B105, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C106" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B106, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B106, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C107" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B107, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B107, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="108" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C108" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B108, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B108, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C109" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B109, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B109, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="110" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C110" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B110, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B110, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C111" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B111, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B111, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="112" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C112" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B112, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B112, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C113" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B113, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B113, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C114" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B114, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B114, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C115" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B115, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B115, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="116" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C116" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B116, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B116, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="117" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C117" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B117, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B117, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="118" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C118" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B118, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B118, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C119" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B119, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B119, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="120" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C120" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B120, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B120, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C121" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B121, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B121, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="122" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C122" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B122, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B122, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C123" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B123, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B123, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="124" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C124" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B124, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B124, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C125" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B125, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B125, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="126" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C126" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B126, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B126, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C127" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B127, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B127, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="128" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C128" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B128, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B128, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C129" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B129, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B129, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="130" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C130" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B130, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B130, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C131" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B131, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B131, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="132" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C132" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B132, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B132, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="133" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C133" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B133, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B133, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="134" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C134" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B134, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B134, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C135" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B135, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B135, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="136" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C136" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B136, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B136, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C137" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B137, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B137, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="138" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C138" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B138, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B138, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C139" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B139, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B139, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="140" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C140" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B140, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B140, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="141" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C141" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B141, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B141, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="142" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C142" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B142, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B142, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C143" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B143, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B143, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="144" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C144" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B144, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B144, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C145" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B145, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B145, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="146" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C146" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B146, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B146, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C147" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B147, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B147, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="148" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C148" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B148, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B148, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C149" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B149, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B149, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="150" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C150" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B150, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B150, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="151" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C151" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B151, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B151, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="152" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C152" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B152, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B152, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="153" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C153" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B153, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B153, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="154" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C154" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B154, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B154, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="155" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C155" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B155, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B155, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="156" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C156" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B156, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B156, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="157" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C157" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B157, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B157, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="158" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C158" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B158, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B158, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="159" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C159" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B159, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B159, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="160" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C160" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B160, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B160, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C161" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B161, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B161, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="162" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C162" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B162, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B162, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C163" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B163, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B163, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="164" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C164" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B164, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B164, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C165" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B165, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B165, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="166" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C166" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B166, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B166, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C167" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B167, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B167, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="168" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C168" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B168, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B168, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="169" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C169" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B169, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B169, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="170" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C170" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B170, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B170, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="171" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C171" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B171, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B171, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="172" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C172" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B172, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B172, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="173" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C173" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B173, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B173, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="174" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C174" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B174, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B174, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="175" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C175" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B175, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B175, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="176" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C176" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B176, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B176, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="177" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C177" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B177, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B177, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="178" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C178" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B178, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B178, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="179" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C179" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B179, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B179, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="180" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C180" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B180, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B180, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="181" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C181" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B181, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B181, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="182" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C182" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B182, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B182, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="183" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C183" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B183, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B183, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="184" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C184" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B184, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B184, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="185" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C185" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B185, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B185, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="186" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C186" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B186, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B186, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="187" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C187" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B187, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B187, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="188" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C188" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B188, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B188, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="189" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C189" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B189, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B189, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="190" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C190" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B190, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B190, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="191" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C191" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B191, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B191, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="192" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C192" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B192, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B192, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="193" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C193" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B193, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B193, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="194" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C194" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B194, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B194, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="195" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C195" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B195, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B195, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="196" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C196" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B196, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B196, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="197" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C197" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B197, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B197, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="198" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C198" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B198, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B198, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="199" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C199" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B199, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B199, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="200" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C200" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$AS$2:$AS$1000000, MATCH(B200, 'Dados Consolidados'!$AR$2:$AR$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$AS$1:$AS$1000000, MATCH(B200, 'Dados Consolidados'!$AR$1:$AR$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -20860,12 +21090,42 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2049" r:id="rId3" name="Button 1">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!ExecutarCadastroSecao">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20EED632-601C-4DD3-90D3-2AD92BB8E994}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20EED632-601C-4DD3-90D3-2AD92BB8E994}">
+  <sheetPr codeName="Planilha8">
     <tabColor theme="2" tint="-0.749992370372631"/>
   </sheetPr>
   <dimension ref="A1:N200"/>
@@ -20873,14 +21133,14 @@
     <sheetView workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.5703125" customWidth="1"/>
     <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="176.28515625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20947,7 +21207,7 @@
     </row>
     <row r="5" spans="1:14" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="40" t="s">
         <v>29</v>
@@ -20961,1165 +21221,1165 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C7" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B7, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B7, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C8" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B8, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B8, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C9" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B9, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B9, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C10" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B10, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B10, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C11" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B11, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B11, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C12" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B12, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B12, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C13" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B13, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B13, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C14" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B14, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B14, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C15" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B15, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B15, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C16" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B16, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B16, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B17, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B17, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B18, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B18, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B19, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B19, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B20, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B20, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B21, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B21, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B22, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B22, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B23, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B23, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B24, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B24, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B25, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B25, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B26, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B26, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B27, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B27, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B28, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B28, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B29, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B29, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B30, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B30, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B31, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B31, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B32, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B32, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B33, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B33, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B34, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B34, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B35, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B35, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B36, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B36, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B37, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B37, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B38, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B38, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B39, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B39, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B40, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B40, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B41, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B41, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B42, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B42, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B43, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B43, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B44, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B44, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B45, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B45, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B46, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B46, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B47, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B47, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B48, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B48, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B49, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B49, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B50, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B50, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B51, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B51, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B52, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B52, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B53, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B53, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B54, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B54, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B55, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B55, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B56, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B56, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B57, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B57, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B58, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B58, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B59, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B59, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B60, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B60, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B61, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B61, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B62, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B62, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B63, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B63, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B64, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B64, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B65, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B65, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B66, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B66, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B67, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B67, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B68, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B68, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B69, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B69, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B70, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B70, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B71, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B71, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B72, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B72, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B73, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B73, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B74, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B74, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B75, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B75, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B76, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B76, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B77, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B77, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B78, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B78, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B79, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B79, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B80, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B80, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B81, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B81, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B82, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B82, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B83, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B83, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B84, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B84, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B85, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B85, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C86" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B86, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B86, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B87, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B87, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C88" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B88, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B88, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B89, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B89, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C90" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B90, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B90, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B91, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B91, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C92" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B92, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B92, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B93, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B93, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C94" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B94, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B94, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B95, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B95, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C96" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B96, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B96, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B97, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B97, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C98" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B98, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B98, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B99, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B99, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C100" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B100, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B100, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B101, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B101, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C102" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B102, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B102, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C103" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B103, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B103, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C104" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B104, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B104, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C105" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B105, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B105, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C106" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B106, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B106, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C107" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B107, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B107, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="108" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C108" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B108, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B108, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C109" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B109, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B109, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="110" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C110" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B110, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B110, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C111" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B111, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B111, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="112" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C112" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B112, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B112, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C113" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B113, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B113, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C114" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B114, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B114, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C115" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B115, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B115, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="116" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C116" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B116, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B116, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="117" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C117" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B117, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B117, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="118" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C118" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B118, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B118, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C119" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B119, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B119, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="120" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C120" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B120, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B120, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C121" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B121, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B121, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="122" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C122" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B122, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B122, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C123" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B123, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B123, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="124" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C124" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B124, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B124, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C125" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B125, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B125, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="126" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C126" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B126, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B126, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C127" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B127, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B127, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="128" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C128" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B128, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B128, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C129" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B129, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B129, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="130" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C130" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B130, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B130, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C131" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B131, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B131, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="132" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C132" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B132, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B132, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="133" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C133" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B133, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B133, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="134" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C134" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B134, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B134, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C135" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B135, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B135, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="136" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C136" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B136, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B136, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C137" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B137, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B137, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="138" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C138" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B138, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B138, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C139" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B139, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B139, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="140" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C140" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B140, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B140, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="141" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C141" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B141, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B141, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="142" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C142" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B142, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B142, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C143" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B143, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B143, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="144" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C144" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B144, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B144, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C145" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B145, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B145, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="146" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C146" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B146, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B146, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C147" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B147, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B147, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="148" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C148" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B148, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B148, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C149" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B149, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B149, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="150" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C150" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B150, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B150, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="151" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C151" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B151, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B151, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="152" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C152" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B152, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B152, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="153" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C153" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B153, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B153, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="154" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C154" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B154, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B154, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="155" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C155" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B155, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B155, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="156" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C156" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B156, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B156, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="157" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C157" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B157, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B157, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="158" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C158" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B158, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B158, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="159" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C159" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B159, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B159, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="160" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C160" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B160, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B160, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C161" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B161, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B161, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="162" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C162" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B162, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B162, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C163" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B163, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B163, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="164" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C164" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B164, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B164, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C165" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B165, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B165, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="166" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C166" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B166, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B166, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C167" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B167, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B167, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="168" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C168" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B168, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B168, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="169" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C169" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B169, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B169, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="170" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C170" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B170, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B170, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="171" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C171" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B171, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B171, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="172" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C172" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B172, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B172, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="173" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C173" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B173, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B173, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="174" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C174" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B174, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B174, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="175" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C175" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B175, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B175, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="176" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C176" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B176, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B176, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="177" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C177" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B177, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B177, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="178" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C178" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B178, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B178, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="179" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C179" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B179, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B179, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="180" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C180" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B180, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B180, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="181" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C181" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B181, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B181, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="182" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C182" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B182, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B182, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="183" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C183" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B183, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B183, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="184" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C184" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B184, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B184, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="185" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C185" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B185, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B185, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="186" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C186" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B186, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B186, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="187" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C187" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B187, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B187, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="188" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C188" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B188, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B188, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="189" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C189" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B189, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B189, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="190" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C190" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B190, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B190, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="191" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C191" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B191, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B191, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="192" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C192" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B192, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B192, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="193" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C193" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B193, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B193, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="194" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C194" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B194, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B194, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="195" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C195" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B195, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B195, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="196" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C196" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B196, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B196, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="197" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C197" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B197, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B197, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="198" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C198" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B198, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B198, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="199" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C199" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B199, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B199, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="200" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C200" s="63" t="e">
-        <f>INT(INDEX('Dados Consolidados'!$R$2:$R$1000000, MATCH(B200, 'Dados Consolidados'!$A$2:$A$1000000, 0)))</f>
+        <f>INT(INDEX('Dados Consolidados'!$R$1:$R$1000000, MATCH(B200, 'Dados Consolidados'!$A$1:$A$1000000, 0)))</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -22134,6 +22394,36 @@
     <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C200" xr:uid="{8771EE18-3FA3-4C4B-BC9E-74C2FA28D036}"/>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="3073" r:id="rId3" name="Button 1">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!ExecutarCadastroEspecie">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
cadastro de atributos funcionando
</commit_message>
<xml_diff>
--- a/Cadastros Auto Nextt limpa.xlsx
+++ b/Cadastros Auto Nextt limpa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Desktop\dev\automacao-nextt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E69404-236C-4383-B41F-79DEEDC8C6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E52C8C-ACEC-4B6B-B6A3-CDE97C55B628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-1950" windowWidth="20730" windowHeight="11040" tabRatio="764" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-1950" windowWidth="20730" windowHeight="11040" tabRatio="764" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nextt" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="75">
   <si>
     <t>Cadastre vários itens simultaneamente</t>
   </si>
@@ -220,12 +220,6 @@
     <t>Estrangeira: adquirida no mercado interno, sem similar nacional, constante em lista de Resolução Camex e gás natural;</t>
   </si>
   <si>
-    <t>Para vincular um atributo a outro, basta relacionar as células correspondentes na grade. Por exemplo, a primeira célula de "Cor" deve estar associada à primeira célula de "Tamanho". Atenção: é essencial que a quantidade de cores seja igual à de tamanhos para garantir a correspondência correta.</t>
-  </si>
-  <si>
-    <t>EM TESTES</t>
-  </si>
-  <si>
     <t>Aviso: Os valores disponíveis para "seção" são importados automaticamente do banco de dados.</t>
   </si>
   <si>
@@ -272,6 +266,9 @@
   </si>
   <si>
     <t>Ao terminar, lembre-se de salvar e importar a planilha Excel para o banco de dados.</t>
+  </si>
+  <si>
+    <t>Para vincular um atributo a outro, basta relacionar as células correspondentes na grade. Por exemplo, a primeira célula de "Cor" deve estar associada à primeira célula de "Tamanho". Atenção: é essencial que a quantidade de cores seja igual à de tamanhos para garantir a correspondência correta. Aviso: é obrigatório preencher pelo menos um atributo por item.</t>
   </si>
 </sst>
 </file>
@@ -577,7 +574,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1029,17 +1026,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFCFCFCF"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FFCFCFCF"/>
@@ -1056,7 +1042,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1300,6 +1286,12 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1381,15 +1373,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -1817,70 +1800,70 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="90"/>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
+      <c r="A4" s="92"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="91"/>
     </row>
     <row r="5" spans="1:15" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="88"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
+      <c r="A5" s="90"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="91"/>
+      <c r="O5" s="91"/>
     </row>
     <row r="6" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="94"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="89"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="89"/>
-      <c r="K6" s="89"/>
-      <c r="L6" s="89"/>
-      <c r="M6" s="89"/>
-      <c r="N6" s="89"/>
-      <c r="O6" s="89"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+      <c r="O6" s="91"/>
     </row>
     <row r="7" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="89"/>
+      <c r="C7" s="91"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="92" t="s">
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="89"/>
-      <c r="I7" s="89"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="91"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -1890,11 +1873,11 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -1907,13 +1890,13 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="89"/>
+      <c r="C9" s="91"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -1926,34 +1909,34 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="89"/>
+      <c r="C10" s="91"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="96" t="s">
-        <v>75</v>
-      </c>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="89"/>
-      <c r="M10" s="89"/>
+      <c r="H10" s="98" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="89"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="89"/>
-      <c r="F11" s="89"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -1969,8 +1952,8 @@
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="89"/>
-      <c r="F12" s="89"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1983,18 +1966,18 @@
     </row>
     <row r="13" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="95" t="s">
+      <c r="B13" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="89"/>
+      <c r="C13" s="91"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="89"/>
-      <c r="F13" s="89"/>
-      <c r="G13" s="92" t="s">
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="94" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="89"/>
-      <c r="I13" s="89"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
@@ -2004,11 +1987,11 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="91"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -2021,60 +2004,60 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="102" t="s">
+      <c r="B15" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="102"/>
+      <c r="C15" s="104"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="103" t="s">
+      <c r="E15" s="91"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="103"/>
-      <c r="I15" s="103"/>
-      <c r="J15" s="103"/>
-      <c r="K15" s="103"/>
-      <c r="L15" s="103"/>
-      <c r="M15" s="103"/>
+      <c r="H15" s="105"/>
+      <c r="I15" s="105"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="105"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="102" t="s">
+      <c r="B16" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="102"/>
+      <c r="C16" s="104"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="103"/>
-      <c r="I16" s="103"/>
-      <c r="J16" s="103"/>
-      <c r="K16" s="103"/>
-      <c r="L16" s="103"/>
-      <c r="M16" s="103"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="91"/>
+      <c r="G16" s="105"/>
+      <c r="H16" s="105"/>
+      <c r="I16" s="105"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="105"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="105"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="102" t="s">
+      <c r="B17" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="102"/>
+      <c r="C17" s="104"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="89"/>
-      <c r="F17" s="89"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="103"/>
-      <c r="I17" s="103"/>
-      <c r="J17" s="103"/>
-      <c r="K17" s="103"/>
-      <c r="L17" s="103"/>
-      <c r="M17" s="103"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="91"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="105"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="105"/>
+      <c r="L17" s="105"/>
+      <c r="M17" s="105"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
@@ -2083,15 +2066,15 @@
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="89"/>
-      <c r="F18" s="89"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="103"/>
-      <c r="I18" s="103"/>
-      <c r="J18" s="103"/>
-      <c r="K18" s="103"/>
-      <c r="L18" s="103"/>
-      <c r="M18" s="103"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="91"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="105"/>
+      <c r="I18" s="105"/>
+      <c r="J18" s="105"/>
+      <c r="K18" s="105"/>
+      <c r="L18" s="105"/>
+      <c r="M18" s="105"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
@@ -2100,15 +2083,15 @@
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="103"/>
-      <c r="H19" s="103"/>
-      <c r="I19" s="103"/>
-      <c r="J19" s="103"/>
-      <c r="K19" s="103"/>
-      <c r="L19" s="103"/>
-      <c r="M19" s="103"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="91"/>
+      <c r="G19" s="105"/>
+      <c r="H19" s="105"/>
+      <c r="I19" s="105"/>
+      <c r="J19" s="105"/>
+      <c r="K19" s="105"/>
+      <c r="L19" s="105"/>
+      <c r="M19" s="105"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
@@ -2117,8 +2100,8 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="89"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="91"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -2134,18 +2117,18 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="89"/>
-      <c r="F21" s="89"/>
-      <c r="G21" s="97" t="s">
+      <c r="E21" s="91"/>
+      <c r="F21" s="91"/>
+      <c r="G21" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="98"/>
-      <c r="I21" s="98"/>
-      <c r="J21" s="98"/>
-      <c r="K21" s="98"/>
-      <c r="L21" s="98"/>
-      <c r="M21" s="98"/>
-      <c r="N21" s="98"/>
+      <c r="H21" s="100"/>
+      <c r="I21" s="100"/>
+      <c r="J21" s="100"/>
+      <c r="K21" s="100"/>
+      <c r="L21" s="100"/>
+      <c r="M21" s="100"/>
+      <c r="N21" s="100"/>
       <c r="O21" s="5"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2153,8 +2136,8 @@
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="89"/>
-      <c r="F22" s="89"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -2170,8 +2153,8 @@
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="89"/>
-      <c r="F23" s="89"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="91"/>
       <c r="G23" s="32" t="s">
         <v>34</v>
       </c>
@@ -2189,8 +2172,8 @@
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="89"/>
-      <c r="F24" s="89"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="91"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -2206,17 +2189,17 @@
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="89"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="91"/>
       <c r="G25" s="33"/>
-      <c r="H25" s="99" t="s">
-        <v>74</v>
-      </c>
-      <c r="I25" s="100"/>
-      <c r="J25" s="100"/>
-      <c r="K25" s="100"/>
-      <c r="L25" s="100"/>
-      <c r="M25" s="100"/>
+      <c r="H25" s="101" t="s">
+        <v>72</v>
+      </c>
+      <c r="I25" s="102"/>
+      <c r="J25" s="102"/>
+      <c r="K25" s="102"/>
+      <c r="L25" s="102"/>
+      <c r="M25" s="102"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
     </row>
@@ -2225,15 +2208,15 @@
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="89"/>
+      <c r="E26" s="91"/>
+      <c r="F26" s="91"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="101"/>
-      <c r="I26" s="101"/>
-      <c r="J26" s="101"/>
-      <c r="K26" s="101"/>
-      <c r="L26" s="101"/>
-      <c r="M26" s="100"/>
+      <c r="H26" s="103"/>
+      <c r="I26" s="103"/>
+      <c r="J26" s="103"/>
+      <c r="K26" s="103"/>
+      <c r="L26" s="103"/>
+      <c r="M26" s="102"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
     </row>
@@ -2242,15 +2225,15 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="89"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="91"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="101"/>
-      <c r="I27" s="101"/>
-      <c r="J27" s="101"/>
-      <c r="K27" s="101"/>
-      <c r="L27" s="101"/>
-      <c r="M27" s="100"/>
+      <c r="H27" s="103"/>
+      <c r="I27" s="103"/>
+      <c r="J27" s="103"/>
+      <c r="K27" s="103"/>
+      <c r="L27" s="103"/>
+      <c r="M27" s="102"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
     </row>
@@ -2259,8 +2242,8 @@
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="89"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="91"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -2276,8 +2259,8 @@
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="89"/>
+      <c r="E29" s="91"/>
+      <c r="F29" s="91"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -2293,8 +2276,8 @@
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="89"/>
+      <c r="E30" s="91"/>
+      <c r="F30" s="91"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -2310,8 +2293,8 @@
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="89"/>
-      <c r="F31" s="89"/>
+      <c r="E31" s="91"/>
+      <c r="F31" s="91"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -2327,8 +2310,8 @@
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="89"/>
+      <c r="E32" s="91"/>
+      <c r="F32" s="91"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -2344,8 +2327,8 @@
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="89"/>
+      <c r="E33" s="91"/>
+      <c r="F33" s="91"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -2361,8 +2344,8 @@
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="89"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="91"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -2378,8 +2361,8 @@
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="89"/>
+      <c r="E35" s="91"/>
+      <c r="F35" s="91"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -2395,8 +2378,8 @@
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="89"/>
-      <c r="F36" s="89"/>
+      <c r="E36" s="91"/>
+      <c r="F36" s="91"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -2412,8 +2395,8 @@
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="89"/>
-      <c r="F37" s="89"/>
+      <c r="E37" s="91"/>
+      <c r="F37" s="91"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -2429,8 +2412,8 @@
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="89"/>
-      <c r="F38" s="89"/>
+      <c r="E38" s="91"/>
+      <c r="F38" s="91"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -2446,8 +2429,8 @@
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="89"/>
-      <c r="F39" s="89"/>
+      <c r="E39" s="91"/>
+      <c r="F39" s="91"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -2463,8 +2446,8 @@
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="89"/>
-      <c r="F40" s="89"/>
+      <c r="E40" s="91"/>
+      <c r="F40" s="91"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -2480,8 +2463,8 @@
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="89"/>
-      <c r="F41" s="89"/>
+      <c r="E41" s="91"/>
+      <c r="F41" s="91"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
@@ -2497,8 +2480,8 @@
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
-      <c r="E42" s="89"/>
-      <c r="F42" s="89"/>
+      <c r="E42" s="91"/>
+      <c r="F42" s="91"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
@@ -2514,8 +2497,8 @@
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
-      <c r="E43" s="89"/>
-      <c r="F43" s="89"/>
+      <c r="E43" s="91"/>
+      <c r="F43" s="91"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
@@ -2531,8 +2514,8 @@
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
-      <c r="E44" s="89"/>
-      <c r="F44" s="89"/>
+      <c r="E44" s="91"/>
+      <c r="F44" s="91"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
@@ -2548,8 +2531,8 @@
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="89"/>
+      <c r="E45" s="91"/>
+      <c r="F45" s="91"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
@@ -2565,8 +2548,8 @@
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
-      <c r="E46" s="89"/>
-      <c r="F46" s="89"/>
+      <c r="E46" s="91"/>
+      <c r="F46" s="91"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
@@ -2582,8 +2565,8 @@
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
-      <c r="E47" s="89"/>
-      <c r="F47" s="89"/>
+      <c r="E47" s="91"/>
+      <c r="F47" s="91"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -2599,8 +2582,8 @@
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
-      <c r="E48" s="89"/>
-      <c r="F48" s="89"/>
+      <c r="E48" s="91"/>
+      <c r="F48" s="91"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
@@ -2616,8 +2599,8 @@
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
-      <c r="E49" s="89"/>
-      <c r="F49" s="89"/>
+      <c r="E49" s="91"/>
+      <c r="F49" s="91"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
@@ -2633,8 +2616,8 @@
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-      <c r="E50" s="89"/>
-      <c r="F50" s="89"/>
+      <c r="E50" s="91"/>
+      <c r="F50" s="91"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
@@ -2687,9 +2670,9 @@
   <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:AG5946"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH2" sqref="AH2"/>
+      <selection pane="bottomLeft" activeCell="AG7" sqref="AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2711,7 +2694,9 @@
     <col min="15" max="15" width="7.7109375" customWidth="1"/>
     <col min="16" max="16" width="43" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="24" width="9.140625" customWidth="1"/>
+    <col min="18" max="20" width="9.140625" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="9.140625" customWidth="1"/>
     <col min="25" max="25" width="9" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="10.85546875" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="7.85546875" hidden="1" customWidth="1"/>
@@ -2720,16 +2705,16 @@
     <col min="30" max="30" width="17.42578125" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="9" hidden="1" customWidth="1"/>
     <col min="32" max="32" width="14" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="0" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -2742,34 +2727,34 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="114" t="s">
+      <c r="Q1" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="106"/>
-      <c r="S1" s="106"/>
-      <c r="T1" s="106"/>
-      <c r="U1" s="106"/>
-      <c r="V1" s="106"/>
-      <c r="W1" s="106"/>
-      <c r="X1" s="115"/>
-      <c r="Y1" s="109" t="s">
+      <c r="R1" s="108"/>
+      <c r="S1" s="108"/>
+      <c r="T1" s="108"/>
+      <c r="U1" s="108"/>
+      <c r="V1" s="108"/>
+      <c r="W1" s="108"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="106"/>
-      <c r="AA1" s="106"/>
-      <c r="AB1" s="106"/>
-      <c r="AC1" s="106"/>
-      <c r="AD1" s="106"/>
-      <c r="AE1" s="106"/>
-      <c r="AF1" s="107"/>
+      <c r="Z1" s="108"/>
+      <c r="AA1" s="108"/>
+      <c r="AB1" s="108"/>
+      <c r="AC1" s="108"/>
+      <c r="AD1" s="108"/>
+      <c r="AE1" s="108"/>
+      <c r="AF1" s="109"/>
     </row>
     <row r="2" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -2782,22 +2767,22 @@
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="89"/>
-      <c r="V2" s="89"/>
-      <c r="W2" s="89"/>
-      <c r="X2" s="116"/>
-      <c r="Y2" s="110"/>
-      <c r="Z2" s="111"/>
-      <c r="AA2" s="111"/>
-      <c r="AB2" s="111"/>
-      <c r="AC2" s="111"/>
-      <c r="AD2" s="111"/>
-      <c r="AE2" s="111"/>
-      <c r="AF2" s="112"/>
+      <c r="Q2" s="91"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="91"/>
+      <c r="U2" s="91"/>
+      <c r="V2" s="91"/>
+      <c r="W2" s="91"/>
+      <c r="X2" s="118"/>
+      <c r="Y2" s="112"/>
+      <c r="Z2" s="113"/>
+      <c r="AA2" s="113"/>
+      <c r="AB2" s="113"/>
+      <c r="AC2" s="113"/>
+      <c r="AD2" s="113"/>
+      <c r="AE2" s="113"/>
+      <c r="AF2" s="114"/>
     </row>
     <row r="3" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
@@ -2848,18 +2833,18 @@
       <c r="P3" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="117" t="s">
+      <c r="Q3" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="R3" s="118"/>
-      <c r="S3" s="118"/>
-      <c r="T3" s="119"/>
-      <c r="U3" s="117" t="s">
+      <c r="R3" s="120"/>
+      <c r="S3" s="120"/>
+      <c r="T3" s="121"/>
+      <c r="U3" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="V3" s="118"/>
-      <c r="W3" s="118"/>
-      <c r="X3" s="119"/>
+      <c r="V3" s="120"/>
+      <c r="W3" s="120"/>
+      <c r="X3" s="121"/>
       <c r="Y3" s="79" t="s">
         <v>10</v>
       </c>
@@ -2926,84 +2911,86 @@
       <c r="P4" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="Q4" s="123" t="s">
-        <v>59</v>
-      </c>
-      <c r="R4" s="124"/>
-      <c r="S4" s="124"/>
-      <c r="T4" s="124"/>
-      <c r="U4" s="124"/>
-      <c r="V4" s="124"/>
-      <c r="W4" s="124"/>
-      <c r="X4" s="125"/>
-      <c r="Y4" s="105" t="s">
+      <c r="Q4" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="V4" s="88"/>
+      <c r="W4" s="88"/>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="Z4" s="106"/>
-      <c r="AA4" s="106"/>
-      <c r="AB4" s="106"/>
-      <c r="AC4" s="106"/>
-      <c r="AD4" s="106"/>
-      <c r="AE4" s="106"/>
-      <c r="AF4" s="107"/>
+      <c r="Z4" s="108"/>
+      <c r="AA4" s="108"/>
+      <c r="AB4" s="108"/>
+      <c r="AC4" s="108"/>
+      <c r="AD4" s="108"/>
+      <c r="AE4" s="108"/>
+      <c r="AF4" s="109"/>
     </row>
     <row r="5" spans="1:33" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5" s="40" t="s">
         <v>49</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F5" s="39"/>
       <c r="G5" s="39"/>
       <c r="H5" s="40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I5" s="38" t="s">
         <v>28</v>
       </c>
       <c r="J5" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="L5" s="40" t="s">
         <v>65</v>
-      </c>
-      <c r="K5" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="L5" s="40" t="s">
-        <v>67</v>
       </c>
       <c r="M5" s="39"/>
       <c r="N5" s="39"/>
       <c r="O5" s="39"/>
       <c r="P5" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q5" s="120" t="s">
-        <v>58</v>
-      </c>
-      <c r="R5" s="121"/>
-      <c r="S5" s="121"/>
-      <c r="T5" s="121"/>
-      <c r="U5" s="121"/>
-      <c r="V5" s="121"/>
-      <c r="W5" s="121"/>
-      <c r="X5" s="122"/>
-      <c r="Y5" s="89"/>
-      <c r="Z5" s="89"/>
-      <c r="AA5" s="89"/>
-      <c r="AB5" s="89"/>
-      <c r="AC5" s="89"/>
-      <c r="AD5" s="89"/>
-      <c r="AE5" s="89"/>
-      <c r="AF5" s="108"/>
+        <v>66</v>
+      </c>
+      <c r="Q5" s="122" t="s">
+        <v>74</v>
+      </c>
+      <c r="R5" s="123"/>
+      <c r="S5" s="123"/>
+      <c r="T5" s="123"/>
+      <c r="U5" s="123"/>
+      <c r="V5" s="123"/>
+      <c r="W5" s="123"/>
+      <c r="X5" s="124"/>
+      <c r="Y5" s="91"/>
+      <c r="Z5" s="91"/>
+      <c r="AA5" s="91"/>
+      <c r="AB5" s="91"/>
+      <c r="AC5" s="91"/>
+      <c r="AD5" s="91"/>
+      <c r="AE5" s="91"/>
+      <c r="AF5" s="110"/>
     </row>
     <row r="6" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
@@ -3036,14 +3023,14 @@
       <c r="V6" s="83"/>
       <c r="W6" s="85"/>
       <c r="X6" s="87"/>
-      <c r="Y6" s="89"/>
-      <c r="Z6" s="89"/>
-      <c r="AA6" s="89"/>
-      <c r="AB6" s="89"/>
-      <c r="AC6" s="89"/>
-      <c r="AD6" s="89"/>
-      <c r="AE6" s="89"/>
-      <c r="AF6" s="108"/>
+      <c r="Y6" s="91"/>
+      <c r="Z6" s="91"/>
+      <c r="AA6" s="91"/>
+      <c r="AB6" s="91"/>
+      <c r="AC6" s="91"/>
+      <c r="AD6" s="91"/>
+      <c r="AE6" s="91"/>
+      <c r="AF6" s="110"/>
     </row>
     <row r="7" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="50"/>
@@ -3102,7 +3089,7 @@
         <v>#N/A</v>
       </c>
       <c r="AG7" s="75" t="str">
-        <f>IF(AND(A7&lt;&gt;"",B7&lt;&gt;"",C7&lt;&gt;"",D7&lt;&gt;"",E7&lt;&gt;"",F7&lt;&gt;"",H7&lt;&gt;"",J7&lt;&gt;"",K7&lt;&gt;"",L7&lt;&gt;"",M7&lt;&gt;"",N7&lt;&gt;"",O7&lt;&gt;"",P7&lt;&gt;""),"OK","n/a")</f>
+        <f>IF(AND(A7&lt;&gt;"",B7&lt;&gt;"",C7&lt;&gt;"",D7&lt;&gt;"",E7&lt;&gt;"",F7&lt;&gt;"",H7&lt;&gt;"",J7&lt;&gt;"",K7&lt;&gt;"",L7&lt;&gt;"",M7&lt;&gt;"",N7&lt;&gt;"",O7&lt;&gt;"",P7&lt;&gt;"", Q7&lt;&gt;"",U7&lt;&gt;""),"OK","n/a")</f>
         <v>n/a</v>
       </c>
     </row>
@@ -3163,7 +3150,7 @@
         <v>#N/A</v>
       </c>
       <c r="AG8" s="75" t="str">
-        <f>IF(AND(A8&lt;&gt;"",B8&lt;&gt;"",C8&lt;&gt;"",D8&lt;&gt;"",E8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;"",J8&lt;&gt;"",K8&lt;&gt;"",L8&lt;&gt;"",M8&lt;&gt;"",N8&lt;&gt;"",O8&lt;&gt;"",P8&lt;&gt;""),"OK","n/a")</f>
+        <f t="shared" ref="AG8:AG71" si="0">IF(AND(A8&lt;&gt;"",B8&lt;&gt;"",C8&lt;&gt;"",D8&lt;&gt;"",E8&lt;&gt;"",F8&lt;&gt;"",H8&lt;&gt;"",J8&lt;&gt;"",K8&lt;&gt;"",L8&lt;&gt;"",M8&lt;&gt;"",N8&lt;&gt;"",O8&lt;&gt;"",P8&lt;&gt;"", Q8&lt;&gt;"",U8&lt;&gt;""),"OK","n/a")</f>
         <v>n/a</v>
       </c>
     </row>
@@ -3224,7 +3211,7 @@
         <v>#N/A</v>
       </c>
       <c r="AG9" s="75" t="str">
-        <f t="shared" ref="AG9:AG72" si="0">IF(AND(A9&lt;&gt;"",B9&lt;&gt;"",C9&lt;&gt;"",D9&lt;&gt;"",E9&lt;&gt;"",F9&lt;&gt;"",H9&lt;&gt;"",J9&lt;&gt;"",K9&lt;&gt;"",L9&lt;&gt;"",M9&lt;&gt;"",N9&lt;&gt;"",O9&lt;&gt;"",P9&lt;&gt;""),"OK","n/a")</f>
+        <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
@@ -7067,7 +7054,7 @@
         <v>#N/A</v>
       </c>
       <c r="AG72" s="75" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AG72:AG135" si="1">IF(AND(A72&lt;&gt;"",B72&lt;&gt;"",C72&lt;&gt;"",D72&lt;&gt;"",E72&lt;&gt;"",F72&lt;&gt;"",H72&lt;&gt;"",J72&lt;&gt;"",K72&lt;&gt;"",L72&lt;&gt;"",M72&lt;&gt;"",N72&lt;&gt;"",O72&lt;&gt;"",P72&lt;&gt;"", Q72&lt;&gt;"",U72&lt;&gt;""),"OK","n/a")</f>
         <v>n/a</v>
       </c>
     </row>
@@ -7128,7 +7115,7 @@
         <v>#N/A</v>
       </c>
       <c r="AG73" s="75" t="str">
-        <f t="shared" ref="AG73:AG136" si="1">IF(AND(A73&lt;&gt;"",B73&lt;&gt;"",C73&lt;&gt;"",D73&lt;&gt;"",E73&lt;&gt;"",F73&lt;&gt;"",H73&lt;&gt;"",J73&lt;&gt;"",K73&lt;&gt;"",L73&lt;&gt;"",M73&lt;&gt;"",N73&lt;&gt;"",O73&lt;&gt;"",P73&lt;&gt;""),"OK","n/a")</f>
+        <f t="shared" si="1"/>
         <v>n/a</v>
       </c>
     </row>
@@ -10971,7 +10958,7 @@
         <v>#N/A</v>
       </c>
       <c r="AG136" s="75" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AG136:AG199" si="2">IF(AND(A136&lt;&gt;"",B136&lt;&gt;"",C136&lt;&gt;"",D136&lt;&gt;"",E136&lt;&gt;"",F136&lt;&gt;"",H136&lt;&gt;"",J136&lt;&gt;"",K136&lt;&gt;"",L136&lt;&gt;"",M136&lt;&gt;"",N136&lt;&gt;"",O136&lt;&gt;"",P136&lt;&gt;"", Q136&lt;&gt;"",U136&lt;&gt;""),"OK","n/a")</f>
         <v>n/a</v>
       </c>
     </row>
@@ -11032,7 +11019,7 @@
         <v>#N/A</v>
       </c>
       <c r="AG137" s="75" t="str">
-        <f t="shared" ref="AG137:AG199" si="2">IF(AND(A137&lt;&gt;"",B137&lt;&gt;"",C137&lt;&gt;"",D137&lt;&gt;"",E137&lt;&gt;"",F137&lt;&gt;"",H137&lt;&gt;"",J137&lt;&gt;"",K137&lt;&gt;"",L137&lt;&gt;"",M137&lt;&gt;"",N137&lt;&gt;"",O137&lt;&gt;"",P137&lt;&gt;""),"OK","n/a")</f>
+        <f t="shared" si="2"/>
         <v>n/a</v>
       </c>
     </row>
@@ -14875,7 +14862,7 @@
         <v>#N/A</v>
       </c>
       <c r="AG200" s="75" t="str">
-        <f>IF(AND(A200&lt;&gt;"",B200&lt;&gt;"",C200&lt;&gt;"",D200&lt;&gt;"",E200&lt;&gt;"",F200&lt;&gt;"",H200&lt;&gt;"",J200&lt;&gt;"",K200&lt;&gt;"",L200&lt;&gt;"",M200&lt;&gt;"",N200&lt;&gt;"",O200&lt;&gt;"",P200&lt;&gt;""),"OK","n/a")</f>
+        <f t="shared" ref="AG200" si="3">IF(AND(A200&lt;&gt;"",B200&lt;&gt;"",C200&lt;&gt;"",D200&lt;&gt;"",E200&lt;&gt;"",F200&lt;&gt;"",H200&lt;&gt;"",J200&lt;&gt;"",K200&lt;&gt;"",L200&lt;&gt;"",M200&lt;&gt;"",N200&lt;&gt;"",O200&lt;&gt;"",P200&lt;&gt;"", Q200&lt;&gt;"",U200&lt;&gt;""),"OK","n/a")</f>
         <v>n/a</v>
       </c>
     </row>
@@ -20684,7 +20671,7 @@
     <row r="5946" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="9">
+  <mergeCells count="8">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="Y4:AF6"/>
     <mergeCell ref="Y1:AF2"/>
@@ -20693,7 +20680,6 @@
     <mergeCell ref="U3:X3"/>
     <mergeCell ref="Q3:T3"/>
     <mergeCell ref="Q5:X5"/>
-    <mergeCell ref="Q4:X4"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <dataValidations count="5">
@@ -20772,12 +20758,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -20790,32 +20776,32 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="114" t="s">
+      <c r="Q1" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="106"/>
-      <c r="S1" s="106"/>
-      <c r="T1" s="106"/>
-      <c r="U1" s="106"/>
-      <c r="V1" s="106"/>
-      <c r="W1" s="106"/>
-      <c r="X1" s="115"/>
-      <c r="Y1" s="109" t="s">
+      <c r="R1" s="108"/>
+      <c r="S1" s="108"/>
+      <c r="T1" s="108"/>
+      <c r="U1" s="108"/>
+      <c r="V1" s="108"/>
+      <c r="W1" s="108"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="106"/>
-      <c r="AA1" s="106"/>
-      <c r="AB1" s="106"/>
-      <c r="AC1" s="106"/>
-      <c r="AD1" s="115"/>
+      <c r="Z1" s="108"/>
+      <c r="AA1" s="108"/>
+      <c r="AB1" s="108"/>
+      <c r="AC1" s="108"/>
+      <c r="AD1" s="117"/>
     </row>
     <row r="2" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
+      <c r="B2" s="126"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -20828,20 +20814,20 @@
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
-      <c r="X2" s="128"/>
-      <c r="Y2" s="110"/>
-      <c r="Z2" s="111"/>
-      <c r="AA2" s="111"/>
-      <c r="AB2" s="111"/>
-      <c r="AC2" s="111"/>
-      <c r="AD2" s="128"/>
+      <c r="Q2" s="112"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="113"/>
+      <c r="X2" s="127"/>
+      <c r="Y2" s="112"/>
+      <c r="Z2" s="113"/>
+      <c r="AA2" s="113"/>
+      <c r="AB2" s="113"/>
+      <c r="AC2" s="113"/>
+      <c r="AD2" s="127"/>
     </row>
     <row r="3" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -20912,14 +20898,14 @@
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
       <c r="X4" s="12"/>
-      <c r="Y4" s="130" t="s">
+      <c r="Y4" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="Z4" s="131"/>
-      <c r="AA4" s="131"/>
-      <c r="AB4" s="131"/>
-      <c r="AC4" s="131"/>
-      <c r="AD4" s="131"/>
+      <c r="Z4" s="130"/>
+      <c r="AA4" s="130"/>
+      <c r="AB4" s="130"/>
+      <c r="AC4" s="130"/>
+      <c r="AD4" s="130"/>
     </row>
     <row r="5" spans="1:30" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
@@ -20946,12 +20932,12 @@
       <c r="V5" s="13"/>
       <c r="W5" s="13"/>
       <c r="X5" s="13"/>
-      <c r="Y5" s="132"/>
-      <c r="Z5" s="132"/>
-      <c r="AA5" s="132"/>
-      <c r="AB5" s="132"/>
-      <c r="AC5" s="132"/>
-      <c r="AD5" s="132"/>
+      <c r="Y5" s="131"/>
+      <c r="Z5" s="131"/>
+      <c r="AA5" s="131"/>
+      <c r="AB5" s="131"/>
+      <c r="AC5" s="131"/>
+      <c r="AD5" s="131"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
@@ -21011,7 +20997,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="188.28515625" customWidth="1"/>
-    <col min="2" max="2" width="154.28515625" style="133" customWidth="1"/>
+    <col min="2" max="2" width="154.28515625" style="132" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -21064,7 +21050,7 @@
     </row>
     <row r="5" spans="1:16" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -21151,7 +21137,7 @@
     </row>
     <row r="5" spans="1:13" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -21185,11 +21171,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="125" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="134" t="s">
+      <c r="B1" s="125"/>
+      <c r="C1" s="133" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="46"/>
@@ -21205,11 +21191,11 @@
       <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="128" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="129"/>
-      <c r="C2" s="134"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="133"/>
       <c r="E2" s="48"/>
       <c r="F2" s="48"/>
       <c r="G2" s="48"/>
@@ -21240,7 +21226,7 @@
       <c r="B4" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="105" t="s">
+      <c r="C4" s="107" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="46"/>
@@ -21250,17 +21236,17 @@
     </row>
     <row r="5" spans="1:15" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="135"/>
+        <v>69</v>
+      </c>
+      <c r="C5" s="134"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="136"/>
-      <c r="B6" s="137"/>
-      <c r="C6" s="135"/>
+      <c r="A6" s="135"/>
+      <c r="B6" s="136"/>
+      <c r="C6" s="134"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7" s="58" t="e">
@@ -22460,11 +22446,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="125" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="134" t="s">
+      <c r="B1" s="125"/>
+      <c r="C1" s="133" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="46"/>
@@ -22479,11 +22465,11 @@
       <c r="N1" s="6"/>
     </row>
     <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="129"/>
-      <c r="C2" s="134"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="133"/>
       <c r="E2" s="48"/>
       <c r="F2" s="48"/>
       <c r="G2" s="49"/>
@@ -22513,7 +22499,7 @@
       <c r="B4" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="105" t="s">
+      <c r="C4" s="107" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="46"/>
@@ -22522,17 +22508,17 @@
     </row>
     <row r="5" spans="1:14" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="135"/>
+        <v>58</v>
+      </c>
+      <c r="C5" s="134"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="136"/>
-      <c r="B6" s="137"/>
-      <c r="C6" s="135"/>
+      <c r="A6" s="135"/>
+      <c r="B6" s="136"/>
+      <c r="C6" s="134"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C7" s="58" t="e">
@@ -23721,7 +23707,7 @@
   <dimension ref="L1:Y8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>